<commit_message>
Remove sample data from template files
</commit_message>
<xml_diff>
--- a/immigration-analytics/src/main/resources/template/Community_Connections.xlsx
+++ b/immigration-analytics/src/main/resources/template/Community_Connections.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="135">
   <si>
     <t xml:space="preserve">Immigration, Refugees and Citizenship Canada
 iCARE - Immigration Contribution Agreement Reporting Environment
@@ -429,75 +429,6 @@
   <si>
     <t xml:space="preserve">Reason for update</t>
   </si>
-  <si>
-    <t xml:space="preserve">[BUID:305939,RID:,ORP:4/5,DTS:2018-08-07 10:05:04][1] (Client) Unable to validate against database. / (Client) Impossible de valider dans la base de données.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOSS/GCMS Client ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12345678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1978-05-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M6G3A4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community centre / library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community-based group events and activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Settlement service provider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Events/visits pertaining to culture or history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversation circle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Access to local community services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community-based group events and activities: Group session (e.g. conversation circles)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Less than 10 people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service ended early (i.e. client ended participation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client felt the service was not meeting current needs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-05-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infant (6-18 months)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Short term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amend record</t>
-  </si>
 </sst>
 </file>
 
@@ -753,7 +684,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BP1004"/>
+  <dimension ref="A1:BP1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
@@ -765,7 +696,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="41.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30.5"/>
@@ -793,7 +724,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="67.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="62.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="44.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="18.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="18.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="24"/>
@@ -1316,209 +1247,75 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>135</v>
-      </c>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="W4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="X4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AD4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AF4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG4" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AH4" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI4" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AJ4" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AK4" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AL4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AM4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AN4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AO4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AP4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AQ4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AR4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AS4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU4" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="AV4" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="AW4" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="AX4" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="AY4" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="AZ4" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA4" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="BB4" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="BC4" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="BD4" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="BE4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="BF4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="BG4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="BH4" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="BI4" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="BJ4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="BK4" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="BL4" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="BM4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="BN4" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="BO4" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="BP4" s="8" t="s">
-        <v>157</v>
-      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="7"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="8"/>
+      <c r="BB4" s="8"/>
+      <c r="BC4" s="8"/>
+      <c r="BD4" s="8"/>
+      <c r="BE4" s="8"/>
+      <c r="BF4" s="8"/>
+      <c r="BG4" s="8"/>
+      <c r="BH4" s="8"/>
+      <c r="BI4" s="8"/>
+      <c r="BJ4" s="8"/>
+      <c r="BK4" s="8"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8"/>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7"/>
@@ -2258,15 +2055,15 @@
       <c r="AI15" s="7"/>
       <c r="AJ15" s="7"/>
       <c r="AK15" s="7"/>
-      <c r="AL15" s="8"/>
-      <c r="AM15" s="8"/>
-      <c r="AN15" s="8"/>
-      <c r="AO15" s="8"/>
-      <c r="AP15" s="8"/>
-      <c r="AQ15" s="8"/>
-      <c r="AR15" s="8"/>
-      <c r="AS15" s="8"/>
-      <c r="AT15" s="8"/>
+      <c r="AL15" s="9"/>
+      <c r="AM15" s="9"/>
+      <c r="AN15" s="9"/>
+      <c r="AO15" s="9"/>
+      <c r="AP15" s="9"/>
+      <c r="AQ15" s="9"/>
+      <c r="AR15" s="9"/>
+      <c r="AS15" s="9"/>
+      <c r="AT15" s="9"/>
       <c r="AU15" s="8"/>
       <c r="AV15" s="8"/>
       <c r="AW15" s="8"/>
@@ -2565,7 +2362,7 @@
       <c r="BJ19" s="8"/>
       <c r="BK19" s="8"/>
       <c r="BL19" s="8"/>
-      <c r="BM19" s="8"/>
+      <c r="BM19" s="9"/>
       <c r="BN19" s="8"/>
       <c r="BO19" s="8"/>
       <c r="BP19" s="8"/>
@@ -2666,13 +2463,13 @@
       <c r="W21" s="8"/>
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="8"/>
-      <c r="AC21" s="8"/>
-      <c r="AD21" s="8"/>
-      <c r="AE21" s="8"/>
-      <c r="AF21" s="8"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="7"/>
@@ -2772,13 +2569,13 @@
       <c r="BG22" s="8"/>
       <c r="BH22" s="8"/>
       <c r="BI22" s="8"/>
-      <c r="BJ22" s="8"/>
+      <c r="BJ22" s="9"/>
       <c r="BK22" s="8"/>
       <c r="BL22" s="8"/>
       <c r="BM22" s="9"/>
       <c r="BN22" s="8"/>
       <c r="BO22" s="8"/>
-      <c r="BP22" s="8"/>
+      <c r="BP22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
@@ -3037,15 +2834,15 @@
       <c r="AR26" s="9"/>
       <c r="AS26" s="9"/>
       <c r="AT26" s="9"/>
-      <c r="AU26" s="8"/>
+      <c r="AU26" s="9"/>
       <c r="AV26" s="8"/>
-      <c r="AW26" s="8"/>
+      <c r="AW26" s="9"/>
       <c r="AX26" s="8"/>
-      <c r="AY26" s="8"/>
+      <c r="AY26" s="9"/>
       <c r="AZ26" s="8"/>
-      <c r="BA26" s="8"/>
+      <c r="BA26" s="9"/>
       <c r="BB26" s="8"/>
-      <c r="BC26" s="8"/>
+      <c r="BC26" s="9"/>
       <c r="BD26" s="8"/>
       <c r="BE26" s="8"/>
       <c r="BF26" s="8"/>
@@ -3057,7 +2854,7 @@
       <c r="BL26" s="8"/>
       <c r="BM26" s="9"/>
       <c r="BN26" s="8"/>
-      <c r="BO26" s="8"/>
+      <c r="BO26" s="9"/>
       <c r="BP26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3071,7 +2868,7 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="K27" s="9"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
@@ -3079,7 +2876,7 @@
       <c r="P27" s="8"/>
       <c r="Q27" s="9"/>
       <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
+      <c r="S27" s="9"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
@@ -3093,7 +2890,7 @@
       <c r="AD27" s="9"/>
       <c r="AE27" s="9"/>
       <c r="AF27" s="9"/>
-      <c r="AG27" s="8"/>
+      <c r="AG27" s="9"/>
       <c r="AH27" s="8"/>
       <c r="AI27" s="7"/>
       <c r="AJ27" s="7"/>
@@ -3110,13 +2907,13 @@
       <c r="AU27" s="9"/>
       <c r="AV27" s="8"/>
       <c r="AW27" s="9"/>
-      <c r="AX27" s="8"/>
+      <c r="AX27" s="9"/>
       <c r="AY27" s="9"/>
-      <c r="AZ27" s="8"/>
+      <c r="AZ27" s="9"/>
       <c r="BA27" s="9"/>
-      <c r="BB27" s="8"/>
+      <c r="BB27" s="9"/>
       <c r="BC27" s="9"/>
-      <c r="BD27" s="8"/>
+      <c r="BD27" s="9"/>
       <c r="BE27" s="8"/>
       <c r="BF27" s="8"/>
       <c r="BG27" s="8"/>
@@ -3145,10 +2942,10 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
+      <c r="O28" s="9"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="9"/>
-      <c r="R28" s="8"/>
+      <c r="R28" s="9"/>
       <c r="S28" s="9"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
@@ -3178,7 +2975,7 @@
       <c r="AS28" s="9"/>
       <c r="AT28" s="9"/>
       <c r="AU28" s="9"/>
-      <c r="AV28" s="8"/>
+      <c r="AV28" s="9"/>
       <c r="AW28" s="9"/>
       <c r="AX28" s="9"/>
       <c r="AY28" s="9"/>
@@ -3216,7 +3013,7 @@
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="8"/>
+      <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
@@ -3225,7 +3022,7 @@
       <c r="V29" s="8"/>
       <c r="W29" s="8"/>
       <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
+      <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
       <c r="AA29" s="9"/>
       <c r="AB29" s="9"/>
@@ -3290,11 +3087,11 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
       <c r="Y30" s="9"/>
       <c r="Z30" s="9"/>
       <c r="AA30" s="9"/>
@@ -3327,9 +3124,9 @@
       <c r="BB30" s="9"/>
       <c r="BC30" s="9"/>
       <c r="BD30" s="9"/>
-      <c r="BE30" s="8"/>
+      <c r="BE30" s="9"/>
       <c r="BF30" s="8"/>
-      <c r="BG30" s="8"/>
+      <c r="BG30" s="9"/>
       <c r="BH30" s="8"/>
       <c r="BI30" s="8"/>
       <c r="BJ30" s="9"/>
@@ -3354,7 +3151,7 @@
       <c r="K31" s="9"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
+      <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
       <c r="Q31" s="9"/>
@@ -3374,7 +3171,7 @@
       <c r="AE31" s="9"/>
       <c r="AF31" s="9"/>
       <c r="AG31" s="9"/>
-      <c r="AH31" s="8"/>
+      <c r="AH31" s="9"/>
       <c r="AI31" s="7"/>
       <c r="AJ31" s="7"/>
       <c r="AK31" s="7"/>
@@ -3490,7 +3287,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
@@ -3702,7 +3499,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
-      <c r="L36" s="8"/>
+      <c r="L36" s="9"/>
       <c r="M36" s="8"/>
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
@@ -4658,7 +4455,7 @@
       <c r="BC49" s="9"/>
       <c r="BD49" s="9"/>
       <c r="BE49" s="9"/>
-      <c r="BF49" s="8"/>
+      <c r="BF49" s="9"/>
       <c r="BG49" s="9"/>
       <c r="BH49" s="8"/>
       <c r="BI49" s="8"/>
@@ -4666,7 +4463,7 @@
       <c r="BK49" s="8"/>
       <c r="BL49" s="8"/>
       <c r="BM49" s="9"/>
-      <c r="BN49" s="8"/>
+      <c r="BN49" s="9"/>
       <c r="BO49" s="9"/>
       <c r="BP49" s="9"/>
     </row>
@@ -5033,7 +4830,7 @@
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
-      <c r="M55" s="8"/>
+      <c r="M55" s="9"/>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
       <c r="P55" s="9"/>
@@ -6008,7 +5805,7 @@
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
+      <c r="H69" s="9"/>
       <c r="I69" s="8"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -7477,7 +7274,7 @@
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
-      <c r="G90" s="8"/>
+      <c r="G90" s="9"/>
       <c r="H90" s="9"/>
       <c r="I90" s="8"/>
       <c r="J90" s="9"/>
@@ -7530,11 +7327,11 @@
       <c r="BE90" s="9"/>
       <c r="BF90" s="9"/>
       <c r="BG90" s="9"/>
-      <c r="BH90" s="8"/>
-      <c r="BI90" s="8"/>
+      <c r="BH90" s="9"/>
+      <c r="BI90" s="9"/>
       <c r="BJ90" s="9"/>
-      <c r="BK90" s="8"/>
-      <c r="BL90" s="8"/>
+      <c r="BK90" s="9"/>
+      <c r="BL90" s="9"/>
       <c r="BM90" s="9"/>
       <c r="BN90" s="9"/>
       <c r="BO90" s="9"/>
@@ -10699,7 +10496,7 @@
       <c r="F136" s="7"/>
       <c r="G136" s="9"/>
       <c r="H136" s="9"/>
-      <c r="I136" s="8"/>
+      <c r="I136" s="9"/>
       <c r="J136" s="9"/>
       <c r="K136" s="9"/>
       <c r="L136" s="9"/>
@@ -40233,7 +40030,7 @@
     <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="7"/>
       <c r="B558" s="7"/>
-      <c r="C558" s="8"/>
+      <c r="C558" s="9"/>
       <c r="D558" s="7"/>
       <c r="E558" s="7"/>
       <c r="F558" s="7"/>
@@ -71450,76 +71247,7 @@
       <c r="BO1003" s="9"/>
       <c r="BP1003" s="9"/>
     </row>
-    <row r="1004" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1004" s="7"/>
-      <c r="B1004" s="7"/>
-      <c r="C1004" s="9"/>
-      <c r="D1004" s="7"/>
-      <c r="E1004" s="7"/>
-      <c r="F1004" s="7"/>
-      <c r="G1004" s="9"/>
-      <c r="H1004" s="9"/>
-      <c r="I1004" s="9"/>
-      <c r="J1004" s="9"/>
-      <c r="K1004" s="9"/>
-      <c r="L1004" s="9"/>
-      <c r="M1004" s="9"/>
-      <c r="N1004" s="9"/>
-      <c r="O1004" s="9"/>
-      <c r="P1004" s="9"/>
-      <c r="Q1004" s="9"/>
-      <c r="R1004" s="9"/>
-      <c r="S1004" s="9"/>
-      <c r="T1004" s="9"/>
-      <c r="U1004" s="9"/>
-      <c r="V1004" s="9"/>
-      <c r="W1004" s="9"/>
-      <c r="X1004" s="9"/>
-      <c r="Y1004" s="9"/>
-      <c r="Z1004" s="9"/>
-      <c r="AA1004" s="9"/>
-      <c r="AB1004" s="9"/>
-      <c r="AC1004" s="9"/>
-      <c r="AD1004" s="9"/>
-      <c r="AE1004" s="9"/>
-      <c r="AF1004" s="9"/>
-      <c r="AG1004" s="9"/>
-      <c r="AH1004" s="9"/>
-      <c r="AI1004" s="7"/>
-      <c r="AJ1004" s="7"/>
-      <c r="AK1004" s="7"/>
-      <c r="AL1004" s="9"/>
-      <c r="AM1004" s="9"/>
-      <c r="AN1004" s="9"/>
-      <c r="AO1004" s="9"/>
-      <c r="AP1004" s="9"/>
-      <c r="AQ1004" s="9"/>
-      <c r="AR1004" s="9"/>
-      <c r="AS1004" s="9"/>
-      <c r="AT1004" s="9"/>
-      <c r="AU1004" s="9"/>
-      <c r="AV1004" s="9"/>
-      <c r="AW1004" s="9"/>
-      <c r="AX1004" s="9"/>
-      <c r="AY1004" s="9"/>
-      <c r="AZ1004" s="9"/>
-      <c r="BA1004" s="9"/>
-      <c r="BB1004" s="9"/>
-      <c r="BC1004" s="9"/>
-      <c r="BD1004" s="9"/>
-      <c r="BE1004" s="9"/>
-      <c r="BF1004" s="9"/>
-      <c r="BG1004" s="9"/>
-      <c r="BH1004" s="9"/>
-      <c r="BI1004" s="9"/>
-      <c r="BJ1004" s="9"/>
-      <c r="BK1004" s="9"/>
-      <c r="BL1004" s="9"/>
-      <c r="BM1004" s="9"/>
-      <c r="BN1004" s="9"/>
-      <c r="BO1004" s="9"/>
-      <c r="BP1004" s="9"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BP1"/>
@@ -71529,91 +71257,91 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C558" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C557" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P4:P29" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P4:P28" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AU4:AU26 AW4:AW26 AY4:AY26 BA4:BA26" type="list">
-      <formula1>#REF!</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AU4:AU25 AW4:AW25 AY4:AY25 BA4:BA25" type="list">
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AV4:AV28 AX4:AX27 AZ4:AZ27 BB4:BB27" type="list">
-      <formula1>#REF!</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AV4:AV27 AX4:AX26 AZ4:AZ26 BB4:BB26" type="list">
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q5:Q28 AL16:AT26 BM20:BM49 Z22:AF27 BJ23:BJ90 BP23:BP26 AL27:AU28 AW27 AY27 BA27 BC27 BO27:BP49 K28:K33 S28 Z28:AG29 AW28:BD28 O29 Q29:S29 AL29:BD30 O30:S30 Y30:AG30 O31:AG31 AL31:BE49 BG31:BG49 N32:AH55 J34:K36 J37:L55 AL50:BG90 BM50:BP90 J56:AH136 H70:H90 G91:H136 AL91:BP1004 G137:AH1004 C559:C1004" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q4:Q27 AL15:AT25 BM19:BM48 Z21:AF26 BJ22:BJ89 BP22:BP25 AL26:AU27 AW26 AY26 BA26 BC26 BO26:BP48 K27:K32 S27 Z27:AG28 AW27:BD27 O28 Q28:S28 AL28:BD29 O29:S29 Y29:AG29 O30:AG30 AL30:BE48 BG30:BG48 N31:AH54 J33:K35 J36:L54 AL49:BG89 BM49:BP89 J55:AH135 H69:H89 G90:H135 AL90:BP1003 G136:AH1003 C558:C1003" type="list">
       <formula1>'xlfile://root/currentdir/[08 community+connections_bulk+upload+template hope.xlsx]lov'!#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H69" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H68" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I4:I136" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I4:I135" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J4:J33" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J4:J32" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K4:K27" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K4:K26" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L4:L36" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L4:L35" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M4:M55" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M4:M54" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N4:N31" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N4:N30" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O4:O28" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O4:O27" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q4:AF4 AL4:AT15 BE4:BG30 BJ4:BJ22 BM4:BM19 R5:AF21 R22:Y27 R28 T28:Y29 T30:X30 BF31:BF49" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R4:AF19 AL4:AT14 BE4:BG29 BJ4:BJ21 BM4:BM18 R20:AF20 R21:Y26 R27 T27:Y28 T29:X29 BF30:BF48" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AG4:AG27" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AG4:AG26" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AH4:AH31" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AH4:AH30" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BC4:BC26" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BC4:BC25" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BD4:BD27" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BD4:BD26" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BN4:BN49" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BN4:BN48" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BO4:BO26" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BO4:BO25" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BP4:BP22" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="BP4:BP21" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4:G90 BH4:BI90 BK4:BL90" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4:G89 BH4:BI89 BK4:BL89" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>